<commit_message>
git config pull.rebase false
</commit_message>
<xml_diff>
--- a/Bugbu 300 BOM.xlsx
+++ b/Bugbu 300 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Royce and Nats\3D Printer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC5C75-DAFE-4943-8EBC-5BC5402BFE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4020EEFA-CD39-420A-97C8-B6581CD46CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{21805C48-AE4E-4274-AFEE-0BBD92515AFF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>MOTION:</t>
   </si>
@@ -71,9 +71,6 @@
     <t>M5 T-slot/T-nut</t>
   </si>
   <si>
-    <t>EXTRUDER</t>
-  </si>
-  <si>
     <t>HEATED BED</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
   </si>
   <si>
     <t>https://github.com/Annex-Engineering/Sherpa_Mini-Extruder</t>
-  </si>
-  <si>
-    <t>3D Printed Sherpa Mini (Print with Printer Parts) Use the STL's and build instructions from the GitHub</t>
   </si>
   <si>
     <t>https://www.aliexpress.us/item/3256803662839179.html?spm=a2g0o.productlist.main.11.77d4So3xSo3xa0&amp;algo_pvid=6e6eb8ef-3d42-4c23-bf20-14358976ad9d&amp;algo_exp_id=6e6eb8ef-3d42-4c23-bf20-14358976ad9d-5&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000027332429742%22%7D&amp;pdp_npi=3%40dis%21USD%2131.93%2130.97%21%21%21%21%21%402100bb6416777106954414139d0729%2112000027332429742%21sea%21US%210&amp;curPageLogUid=cpJxAMdvL2Ar</t>
@@ -266,6 +260,24 @@
       <t>:  The items listed don't include any extra wiring or a Pi and as with any BOM, there are going to be small miscellaneous parts needed along the way.  The scew assortments will hopefully cover a lot of the miscellaneous.  For a more rigid gantry, 4 - 45mm Linear Bearings are better, but the shorter ones in the BOM will work fine.  This list is only a guide, better pricing may be found elsewhere.  While every effort has been made to make this a complete list, and the design easy to assemble, please know this is still a self sourced ground up 3D printer build and will require printed parts, time, and attention to details.  All work is done so at your own risk and without any liability to the designer of the project.
 The STL file parts are pre orientated for best printing.  Print with no less than 6 walls and 20% infill.  The STL file name will tell you quantity of each item and if it needs supports, only two parts should need supports.  I use Polymaker PLA Pro for the parts unless I enclose the printer, I go to Polymaker ASA or ABS.</t>
     </r>
+  </si>
+  <si>
+    <t>EXTRUDER: Note that my design can accommodate a few designs, select which one you want to use, just note you will need a different gear kit for the Hummbingbird Extruder</t>
+  </si>
+  <si>
+    <t>3D Printed Sherpa Mini (Print parts and assemble) Use the STL's and build instructions from the GitHub</t>
+  </si>
+  <si>
+    <t>3D Printed Vorxtrudort (Print parts and assemble) Use the STL's and build instructions from the GitHub</t>
+  </si>
+  <si>
+    <t>3D Printed Hummingbird (Print parts and assemble.  Order big gear kit from Github link) Use the STL's and build instructions from the GitHub</t>
+  </si>
+  <si>
+    <t>https://github.com/nhchiu/VoronMods/tree/main/Extruders/Vorxtrudort</t>
+  </si>
+  <si>
+    <t>https://github.com/nhchiu/VoronMods/tree/main/Extruders/Hummingbird</t>
   </si>
 </sst>
 </file>
@@ -356,12 +368,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,6 +379,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -686,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF676DE-F0D5-422E-B84F-2D590F041400}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,25 +720,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -738,13 +756,13 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -756,8 +774,8 @@
         <f>PRODUCT(B4:C4)</f>
         <v>9</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>25</v>
+      <c r="E4" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -771,14 +789,14 @@
         <v>1.2</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D41" si="0">PRODUCT(B5:C5)</f>
+        <f t="shared" ref="D5:D43" si="0">PRODUCT(B5:C5)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -792,11 +810,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -810,13 +828,13 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -828,13 +846,13 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -846,13 +864,13 @@
         <f t="shared" si="0"/>
         <v>36.75</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -864,11 +882,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -882,11 +900,11 @@
         <f t="shared" si="0"/>
         <v>24.75</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -900,13 +918,13 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -918,13 +936,13 @@
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -936,8 +954,8 @@
         <f t="shared" si="0"/>
         <v>5.0400000000000009</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>67</v>
+      <c r="E14" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -946,6 +964,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -956,10 +975,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -971,11 +991,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -989,13 +1009,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1007,13 +1027,13 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1025,13 +1045,13 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -1043,13 +1063,13 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1061,13 +1081,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1079,8 +1099,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E23" t="s">
-        <v>58</v>
+      <c r="E23" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,20 +1109,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>11</v>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1114,230 +1136,254 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>44</v>
+      <c r="E26" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>60</v>
+      <c r="A27" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5">
+        <v>25</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5">
+        <v>12</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5">
+        <v>16</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>24</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>40</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5">
+        <v>31</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
-      <c r="D28" s="5">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5">
+        <v>22</v>
+      </c>
+      <c r="D40" s="5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5">
+        <v>9</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5">
+        <v>9</v>
+      </c>
+      <c r="D42" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5">
-        <v>25</v>
-      </c>
-      <c r="D30" s="5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5">
-        <v>12</v>
-      </c>
-      <c r="D31" s="5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
-      <c r="D32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5">
-        <v>16</v>
-      </c>
-      <c r="D34" s="5">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5">
-        <v>24</v>
-      </c>
-      <c r="D35" s="5">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="E35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="5">
-        <v>40</v>
-      </c>
-      <c r="D36" s="5">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5">
-        <v>31</v>
-      </c>
-      <c r="D37" s="5">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5">
-        <v>22</v>
-      </c>
-      <c r="D38" s="5">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5">
-        <v>9</v>
-      </c>
-      <c r="D39" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" s="5">
-        <v>9</v>
-      </c>
-      <c r="D40" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5">
-        <f>SUM(D4:D41)</f>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5">
+        <f>SUM(D4:D43)</f>
         <v>453.03999999999996</v>
       </c>
     </row>
@@ -1363,16 +1409,16 @@
     <hyperlink ref="E4" r:id="rId14" xr:uid="{07A45856-D2D0-4FFF-97C9-E3555BCFAA8B}"/>
     <hyperlink ref="E20" r:id="rId15" xr:uid="{56C5960E-2BF9-46E2-8317-7E0F658A70AE}"/>
     <hyperlink ref="E26" r:id="rId16" xr:uid="{D03C535B-7CC8-411C-8A28-04C458EE9D58}"/>
-    <hyperlink ref="E30" r:id="rId17" display="https://www.amazon.com/Ender-V2-Heated-Bed-Replacement/dp/B08VHTW8CQ/ref=sr_1_1_sspa?keywords=ender+3+24v+heated+bed&amp;qid=1676582719&amp;sprefix=ender+3+24v+hea%2Caps%2C149&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExQjRXTFBEVzlON0ZIJmVuY3J5cHRlZElkPUEwODY2MjI3MjhIVkxDODZEUUk4UyZlbmNyeXB0ZWRBZElkPUEwMzMxNDM0M1RBNkM2UDRIV01IWCZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{AB5F90A7-ACFD-4B79-893F-3A1DEDC02D95}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{EFDF3B74-F1A3-4159-9B06-1C3B11A5F217}"/>
-    <hyperlink ref="E36" r:id="rId19" display="https://www.amazon.com/BIGTREETECH-Upgrade-Control-TMC2209-Creality/dp/B0882QGFZR/ref=sr_1_1_sspa?crid=WGO9880SJLPG&amp;keywords=bbt+skr+mini+e3&amp;qid=1676582979&amp;sprefix=bbt+skr+mini+e3%2Caps%2C132&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFQWDA4RVRFNFhGR00mZW5jcnlwdGVkSWQ9QTAwMTk0OTROOFdVWVhEWDdBRjcmZW5jcnlwdGVkQWRJZD1BMDA2MjM2MTFLUVE1UzUwVU5GUlMmd2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl" xr:uid="{273878EE-6845-4CDB-AF7A-51536BE5E383}"/>
-    <hyperlink ref="E38" r:id="rId20" xr:uid="{20493BE6-04E4-4B11-83C9-53420756DEAE}"/>
-    <hyperlink ref="E39" r:id="rId21" xr:uid="{83BE0DAF-4C5D-4354-ABBF-BE30AB992DD6}"/>
-    <hyperlink ref="E40" r:id="rId22" xr:uid="{4DD2E72C-2174-4C13-ABFB-48DC73474564}"/>
+    <hyperlink ref="E32" r:id="rId17" display="https://www.amazon.com/Ender-V2-Heated-Bed-Replacement/dp/B08VHTW8CQ/ref=sr_1_1_sspa?keywords=ender+3+24v+heated+bed&amp;qid=1676582719&amp;sprefix=ender+3+24v+hea%2Caps%2C149&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUExQjRXTFBEVzlON0ZIJmVuY3J5cHRlZElkPUEwODY2MjI3MjhIVkxDODZEUUk4UyZlbmNyeXB0ZWRBZElkPUEwMzMxNDM0M1RBNkM2UDRIV01IWCZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=" xr:uid="{AB5F90A7-ACFD-4B79-893F-3A1DEDC02D95}"/>
+    <hyperlink ref="E33" r:id="rId18" xr:uid="{EFDF3B74-F1A3-4159-9B06-1C3B11A5F217}"/>
+    <hyperlink ref="E38" r:id="rId19" display="https://www.amazon.com/BIGTREETECH-Upgrade-Control-TMC2209-Creality/dp/B0882QGFZR/ref=sr_1_1_sspa?crid=WGO9880SJLPG&amp;keywords=bbt+skr+mini+e3&amp;qid=1676582979&amp;sprefix=bbt+skr+mini+e3%2Caps%2C132&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFQWDA4RVRFNFhGR00mZW5jcnlwdGVkSWQ9QTAwMTk0OTROOFdVWVhEWDdBRjcmZW5jcnlwdGVkQWRJZD1BMDA2MjM2MTFLUVE1UzUwVU5GUlMmd2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl" xr:uid="{273878EE-6845-4CDB-AF7A-51536BE5E383}"/>
+    <hyperlink ref="E40" r:id="rId20" xr:uid="{20493BE6-04E4-4B11-83C9-53420756DEAE}"/>
+    <hyperlink ref="E41" r:id="rId21" xr:uid="{83BE0DAF-4C5D-4354-ABBF-BE30AB992DD6}"/>
+    <hyperlink ref="E42" r:id="rId22" xr:uid="{4DD2E72C-2174-4C13-ABFB-48DC73474564}"/>
     <hyperlink ref="E13" r:id="rId23" display="https://www.aliexpress.us/item/2251832113069399.html?spm=a2g0o.productlist.main.53.3694S3j7S3j75k&amp;algo_pvid=ce75d9de-6b64-46a1-b338-9b8c2b0f787a&amp;algo_exp_id=ce75d9de-6b64-46a1-b338-9b8c2b0f787a-26&amp;pdp_ext_f=%7B%22sku_id%22%3A%2210000003969762805%22%7D&amp;pdp_npi=3%40dis%21USD%211.99%211.99%21%21%21%21%21%40211bd8be16777098448855150d06df%2110000003969762805%21sea%21US%210&amp;curPageLogUid=Sgd0cwKojbJx" xr:uid="{DC308216-1629-4D8B-B0A2-A64CD7AD1F2E}"/>
     <hyperlink ref="E27" r:id="rId24" xr:uid="{90A16F8B-A884-4992-9699-D1235A2EFEB7}"/>
-    <hyperlink ref="E37" r:id="rId25" display="https://www.aliexpress.us/item/3256803662839179.html?spm=a2g0o.productlist.main.11.77d4So3xSo3xa0&amp;algo_pvid=6e6eb8ef-3d42-4c23-bf20-14358976ad9d&amp;algo_exp_id=6e6eb8ef-3d42-4c23-bf20-14358976ad9d-5&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000027332429742%22%7D&amp;pdp_npi=3%40dis%21USD%2131.93%2130.97%21%21%21%21%21%402100bb6416777106954414139d0729%2112000027332429742%21sea%21US%210&amp;curPageLogUid=cpJxAMdvL2Ar" xr:uid="{AE4B8A3C-5D82-4200-9738-C3536CD044E0}"/>
-    <hyperlink ref="E34" r:id="rId26" xr:uid="{66C7EC23-F307-4900-9715-21B056EA6042}"/>
+    <hyperlink ref="E39" r:id="rId25" display="https://www.aliexpress.us/item/3256803662839179.html?spm=a2g0o.productlist.main.11.77d4So3xSo3xa0&amp;algo_pvid=6e6eb8ef-3d42-4c23-bf20-14358976ad9d&amp;algo_exp_id=6e6eb8ef-3d42-4c23-bf20-14358976ad9d-5&amp;pdp_ext_f=%7B%22sku_id%22%3A%2212000027332429742%22%7D&amp;pdp_npi=3%40dis%21USD%2131.93%2130.97%21%21%21%21%21%402100bb6416777106954414139d0729%2112000027332429742%21sea%21US%210&amp;curPageLogUid=cpJxAMdvL2Ar" xr:uid="{AE4B8A3C-5D82-4200-9738-C3536CD044E0}"/>
+    <hyperlink ref="E36" r:id="rId26" xr:uid="{66C7EC23-F307-4900-9715-21B056EA6042}"/>
     <hyperlink ref="E14" r:id="rId27" xr:uid="{1A54B1EA-EEB5-4297-8AFC-8219A17B20AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>